<commit_message>
Mapa de procesos V3.0.0
</commit_message>
<xml_diff>
--- a/DOCUMENTACIÓN/ELICITACION/10. Mapa de Procesos/G1_MAPA_PROC_10N_14569_V3.0.0.xlsx
+++ b/DOCUMENTACIÓN/ELICITACION/10. Mapa de Procesos/G1_MAPA_PROC_10N_14569_V3.0.0.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\SEPTIMO SEMESTRE MAYO 24 - SEPTIEMBRE 24\14569 ING REQUISITOS SW\PullaguariAxel_14569__G1_IR\DOCUMENTACIÓN\ELICITACION\10. Mapa de Procesos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80F6B6D8-D8D6-47C2-824E-5EA008E8BE3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B527EC26-D69B-4B1D-B19C-648AA9479D46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{4997B183-6BA5-427C-8615-A6F9FCD80629}"/>
   </bookViews>
@@ -2693,7 +2693,7 @@
           </a:r>
           <a:r>
             <a:rPr lang="es-EC"/>
-            <a:t>El administrador o asistente debe acceder manualmente a la cuenta bancaria para verificar la recepción del pago, confirmar que los detalles de la transferencia coincidan con la información del cliente, registrar la confirmación en un libro de contabilidad, e informar al equipo de preparación que el pago ha sido recibido.</a:t>
+            <a:t>El administrador debe acceder manualmente a la cuenta bancaria para verificar la recepción del pago, confirmar que los detalles de la transferencia coincidan con la información del cliente, registrar la confirmación en un libro de contabilidad, e informar al equipo de preparación que el pago ha sido recibido.</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -2704,7 +2704,15 @@
           </a:r>
           <a:r>
             <a:rPr lang="es-EC"/>
-            <a:t>El administrador debe revisar manualmente la lista de productos solicitados por el cliente, comparar cada producto preparado con la lista de solicitud, utilizar una lista de verificación impresa y marcar cada producto como "correcto", realizar una doble confirmación por otro miembro del equipo, y registrar y firmar la lista antes del envío.</a:t>
+            <a:t>El administrador debe revisar manualmente la lista de productos solicitados por el cliente, comparar cada producto preparado con la lista de solicitud, utilizar una lista de verificación impresa y marcar cada producto como "correcto", y realizar una doble confirmación</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-EC" baseline="0"/>
+            <a:t> con su asistente</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-EC"/>
+            <a:t>.</a:t>
           </a:r>
           <a:endParaRPr lang="es-EC" sz="1100"/>
         </a:p>
@@ -7506,8 +7514,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="4636666" y="7027906"/>
-          <a:ext cx="841752" cy="950405"/>
+          <a:off x="4654453" y="6975858"/>
+          <a:ext cx="848866" cy="941980"/>
           <a:chOff x="9484702" y="2765066"/>
           <a:chExt cx="1089646" cy="1074767"/>
         </a:xfrm>
@@ -7964,8 +7972,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="13126994" y="6871386"/>
-          <a:ext cx="818891" cy="947830"/>
+          <a:off x="13183910" y="6819338"/>
+          <a:ext cx="826006" cy="941090"/>
           <a:chOff x="9484702" y="2765066"/>
           <a:chExt cx="1089646" cy="1074767"/>
         </a:xfrm>
@@ -9413,7 +9421,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CAE3A4D-6C57-42F5-813D-06E56D78CC84}">
   <dimension ref="A2:BA62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="74" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="E35" zoomScale="110" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B2" sqref="B2:AG4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Cambios Mapa de procesos
</commit_message>
<xml_diff>
--- a/DOCUMENTACIÓN/ELICITACION/10. Mapa de Procesos/G1_MAPA_PROC_10N_14569_V3.0.0.xlsx
+++ b/DOCUMENTACIÓN/ELICITACION/10. Mapa de Procesos/G1_MAPA_PROC_10N_14569_V3.0.0.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\SEPTIMO SEMESTRE MAYO 24 - SEPTIEMBRE 24\14569 ING REQUISITOS SW\PullaguariAxel_14569__G1_IR\DOCUMENTACIÓN\ELICITACION\10. Mapa de Procesos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B527EC26-D69B-4B1D-B19C-648AA9479D46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84235867-9D64-4B8E-B0C6-3F0F21D98286}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{4997B183-6BA5-427C-8615-A6F9FCD80629}"/>
   </bookViews>
@@ -1324,7 +1324,7 @@
               </a:solidFill>
               <a:latin typeface="Aptos Narrow" panose="020B0004020202020204" pitchFamily="34" charset="0"/>
             </a:rPr>
-            <a:t>8.Recibier</a:t>
+            <a:t>8.Recibir</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
@@ -2476,7 +2476,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>628952</xdr:colOff>
+      <xdr:colOff>710338</xdr:colOff>
       <xdr:row>57</xdr:row>
       <xdr:rowOff>72572</xdr:rowOff>
     </xdr:to>
@@ -2496,8 +2496,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2273905" y="9869714"/>
-          <a:ext cx="2346476" cy="1995715"/>
+          <a:off x="2227165" y="9578198"/>
+          <a:ext cx="2357749" cy="2131018"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst/>
@@ -2579,6 +2579,32 @@
             </a:rPr>
             <a:t>utilizada para recibir y gestionar los comentarios y valoraciones de los clientes.</a:t>
           </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Orden de preparación:</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> Paso a paso para la elaboración del producto</a:t>
+          </a:r>
           <a:endParaRPr lang="es-MX">
             <a:effectLst/>
           </a:endParaRPr>
@@ -2594,7 +2620,31 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>Guía de Envío: Información de envío del producto.</a:t>
+            <a:t>Orden de Envío: Paso</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> a paso para el</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> envío del producto.</a:t>
           </a:r>
           <a:endParaRPr lang="es-MX">
             <a:effectLst/>
@@ -7514,8 +7564,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="4654453" y="6975858"/>
-          <a:ext cx="848866" cy="941980"/>
+          <a:off x="4649756" y="6973627"/>
+          <a:ext cx="846988" cy="940806"/>
           <a:chOff x="9484702" y="2765066"/>
           <a:chExt cx="1089646" cy="1074767"/>
         </a:xfrm>
@@ -7972,8 +8022,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="13183910" y="6819338"/>
-          <a:ext cx="826006" cy="941090"/>
+          <a:off x="13168881" y="6817107"/>
+          <a:ext cx="824128" cy="940151"/>
           <a:chOff x="9484702" y="2765066"/>
           <a:chExt cx="1089646" cy="1074767"/>
         </a:xfrm>
@@ -9421,8 +9471,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CAE3A4D-6C57-42F5-813D-06E56D78CC84}">
   <dimension ref="A2:BA62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E35" zoomScale="110" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:AG4"/>
+    <sheetView tabSelected="1" topLeftCell="B18" zoomScale="59" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J41" sqref="J41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.33203125" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>